<commit_message>
Change variable and argument names
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adriane.pedroso\Documents\UiPath\Calculate_Client_Security\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9898D7ED-0D14-40B3-B235-91A040EA42AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3A4685-F820-4280-B468-BD4E2A1DF32C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>